<commit_message>
sleep more to get homepage
</commit_message>
<xml_diff>
--- a/dataset_2022/dataset_Vitas_plus_large.xlsx
+++ b/dataset_2022/dataset_Vitas_plus_large.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etemp\IoT\6-VUI_problem\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etemp\IoT\4-Elevate\GPT4_vitas\dataset_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D464C68D-D16E-4098-868B-5E11C7B5E733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A772A6-4A56-4C12-ABCC-4993345FCEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="520" windowWidth="15110" windowHeight="14750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="520" windowWidth="15110" windowHeight="14750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elevate(large)" sheetId="1" r:id="rId1"/>
@@ -7419,7 +7419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
@@ -10900,8 +10900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>

</xml_diff>